<commit_message>
Delete old version of Fiscal_data_EU.xlsx and add new version
</commit_message>
<xml_diff>
--- a/app/data/Fiscal_data_EU.xlsx
+++ b/app/data/Fiscal_data_EU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kogimandias/DataScience/euro_law/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1E4B23-791B-2848-B166-6B82F1F153E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A2B446-7F5F-B246-A3FD-96C108BAB15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" xr2:uid="{D56591AB-A7F4-F643-A985-80CEC621DBC0}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="138">
   <si>
     <t>Country</t>
   </si>
@@ -417,38 +417,53 @@
     <t>https://www.careersinpoland.com/article/news/poland-introduces-a-new-12-tax-rate-for-it-specialists</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.oecd.org/tax/tax-policy/corporate-tax-statistics-belgium.pdf </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://taxsummaries.pwc.com/bulgaria/corporate/taxes-on-corporate-income </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://taxsummaries.pwc.com/hungary/corporate/taxes-on-corporate-income </t>
-  </si>
-  <si>
     <t>https://taxsummaries.pwc.com/ireland/corporate/taxes-on-corporate-income</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://www.ey.com/en_gl/tax-guides/worldwide-corporate-tax-guide-2022</t>
+    <t>0.20</t>
+  </si>
+  <si>
+    <t>https://www.oecd.org/tax/tax-policy/corporate-tax-statistics-belgium.pdf</t>
+  </si>
+  <si>
+    <t>0.10</t>
+  </si>
+  <si>
+    <t>https://taxsummaries.pwc.com/bulgaria/corporate/taxes-on-corporate-income</t>
+  </si>
+  <si>
+    <t>0.03</t>
+  </si>
+  <si>
+    <t>0.13</t>
+  </si>
+  <si>
+    <t>https://www.ey.com/en_gl/tax-guides/worldwide-corporate-tax-guide-2022</t>
+  </si>
+  <si>
+    <t>0.30</t>
+  </si>
+  <si>
+    <t>https://taxsummaries.pwc.com/hungary/corporate/taxes-on-corporate-income</t>
+  </si>
+  <si>
+    <t>0.28</t>
+  </si>
+  <si>
+    <t>0.32</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -458,22 +473,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -481,38 +502,19 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -851,14 +853,14 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="D16" sqref="A1:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="10.83203125" style="1"/>
     <col min="4" max="4" width="74.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="113.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -870,7 +872,7 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -881,474 +883,493 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="4" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D5" t="s">
-        <v>100</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D9" t="s">
-        <v>66</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D26" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D11" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" t="s">
-        <v>86</v>
-      </c>
-      <c r="D12" t="s">
-        <v>69</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D13" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" t="s">
-        <v>94</v>
-      </c>
-      <c r="D14" t="s">
-        <v>71</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" t="s">
-        <v>85</v>
-      </c>
-      <c r="D15" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" t="s">
-        <v>90</v>
-      </c>
-      <c r="D17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" t="s">
-        <v>75</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" t="s">
-        <v>95</v>
-      </c>
-      <c r="D19" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" t="s">
-        <v>101</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" t="s">
-        <v>78</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" t="s">
-        <v>102</v>
-      </c>
-      <c r="D22" t="s">
-        <v>103</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" t="s">
-        <v>96</v>
-      </c>
-      <c r="D23" t="s">
-        <v>79</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24" t="s">
-        <v>91</v>
-      </c>
-      <c r="D24" t="s">
-        <v>80</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="D27" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D25" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D26" t="s">
-        <v>82</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" t="s">
-        <v>83</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" t="s">
-        <v>99</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="D28" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="2" t="s">
         <v>89</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E20" r:id="rId1" xr:uid="{BCFA27AA-0BF1-D046-B6FD-65445C04210B}"/>
-    <hyperlink ref="E22" r:id="rId2" xr:uid="{E183EA0B-C7C9-7342-9E81-D564D0CA4CFC}"/>
-    <hyperlink ref="E5" r:id="rId3" xr:uid="{F3DFA55F-1DD9-3C48-BBCD-9758E5AD69AB}"/>
-    <hyperlink ref="E3" r:id="rId4" xr:uid="{CFE22708-2BFF-D440-8C4D-3B15498C925B}"/>
-    <hyperlink ref="E4" r:id="rId5" xr:uid="{B81ED8B4-CE7F-A544-AF8F-BA88B78F1CA9}"/>
-    <hyperlink ref="E14" r:id="rId6" xr:uid="{186D2551-5FA2-4C4E-A642-6D26400478C8}"/>
-    <hyperlink ref="E15" r:id="rId7" xr:uid="{4494FB7D-AF08-E54F-8F2B-552E972C0CA9}"/>
-    <hyperlink ref="E2:E28" r:id="rId8" display="https://taxfoundation.org/2022-corporate-tax-rates-in-europe/" xr:uid="{1D99B4B1-8653-004F-AA68-369B3053AB27}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{4E562E5E-8003-9D46-BF8B-0736E20EABDB}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{7E22BD00-EAFE-AA49-B82D-30C56B3DDC87}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{56D5F771-BF5F-B74B-906D-331566A672EC}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{A9ED6907-2129-9244-A32D-845C46BDC57D}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{908744CC-A17F-4E46-85F4-B8A0456E554A}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{5CD9B5DA-DEFC-3B48-BE73-95E663B108A8}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{D69F4408-6317-6342-AFB6-84A82A08545F}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{56D684F6-5B7E-B64F-9E77-43BE3D0C050B}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{E83FC587-E28F-4A4A-AC90-8432D50FE413}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{55C2FD93-F9FC-B545-BF9E-AEDD3C57943C}"/>
+    <hyperlink ref="E12" r:id="rId11" xr:uid="{F1DC58D0-2F43-0A49-8A68-305BC2512A07}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{D6ACE2C2-87A6-6A48-9442-20B2517B410D}"/>
+    <hyperlink ref="E14" r:id="rId13" xr:uid="{CABED5B3-E0A7-5342-9C8A-C5E7C05E0F97}"/>
+    <hyperlink ref="E15" r:id="rId14" xr:uid="{B3075F04-23B5-FA4A-A6C1-02441F65C517}"/>
+    <hyperlink ref="E16" r:id="rId15" xr:uid="{D50E49FC-C894-1543-9098-287B2E806F06}"/>
+    <hyperlink ref="E17" r:id="rId16" xr:uid="{C525074A-F9A2-F343-B1AE-3EE8C9FA4579}"/>
+    <hyperlink ref="E18" r:id="rId17" xr:uid="{796070E8-D873-8C4C-B757-D406C317AD41}"/>
+    <hyperlink ref="E19" r:id="rId18" xr:uid="{F85B930A-AA65-4247-B54F-A14564041E69}"/>
+    <hyperlink ref="E20" r:id="rId19" xr:uid="{BFB779AE-B5A6-1746-B4E1-CA5D09649D87}"/>
+    <hyperlink ref="E21" r:id="rId20" xr:uid="{4FA3BD5C-3750-F24C-A00F-C702768452A6}"/>
+    <hyperlink ref="E22" r:id="rId21" xr:uid="{9E5ADB4D-4C2B-F84D-9217-5D634A534082}"/>
+    <hyperlink ref="E23" r:id="rId22" xr:uid="{91BEE282-729D-FB4A-972C-446F3853BB2D}"/>
+    <hyperlink ref="E24" r:id="rId23" xr:uid="{DE17B514-D857-834B-8247-DB78D70F2B06}"/>
+    <hyperlink ref="E25" r:id="rId24" xr:uid="{398018A7-D0FF-B14D-9168-A734ADCF58DC}"/>
+    <hyperlink ref="E26" r:id="rId25" xr:uid="{E0F64863-51B2-684E-BC84-EB11F0ED4679}"/>
+    <hyperlink ref="E27" r:id="rId26" xr:uid="{2E731C9D-4B24-F746-B8DA-103EB8E68F68}"/>
+    <hyperlink ref="E28" r:id="rId27" xr:uid="{F12464FA-8CBA-A843-AE7A-AEC341877029}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add country selection sidebar and display tax details
</commit_message>
<xml_diff>
--- a/app/data/Fiscal_data_EU.xlsx
+++ b/app/data/Fiscal_data_EU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kogimandias/DataScience/euro_law/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A2B446-7F5F-B246-A3FD-96C108BAB15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5BBCA1-A672-EE4A-9C13-A46DA2673716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" xr2:uid="{D56591AB-A7F4-F643-A985-80CEC621DBC0}"/>
   </bookViews>
@@ -507,7 +507,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -515,6 +515,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -853,7 +863,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="A1:E28"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -861,7 +871,7 @@
     <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="1"/>
-    <col min="4" max="4" width="74.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="74.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="113.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -875,41 +885,41 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="27" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="7" t="s">
         <v>60</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="27" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="7" t="s">
         <v>61</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -923,27 +933,27 @@
       <c r="B4" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="7" t="s">
         <v>62</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="40" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="7" t="s">
         <v>100</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -957,10 +967,10 @@
       <c r="B6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="7" t="s">
         <v>63</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -974,10 +984,10 @@
       <c r="B7" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="7" t="s">
         <v>64</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -991,27 +1001,27 @@
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="7" t="s">
         <v>65</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="27" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="7" t="s">
         <v>66</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -1025,27 +1035,27 @@
       <c r="B10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="7" t="s">
         <v>67</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="27" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="7" t="s">
         <v>68</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -1059,10 +1069,10 @@
       <c r="B12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="7" t="s">
         <v>69</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -1076,10 +1086,10 @@
       <c r="B13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="7" t="s">
         <v>70</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -1093,10 +1103,10 @@
       <c r="B14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="7" t="s">
         <v>71</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -1110,10 +1120,10 @@
       <c r="B15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="7" t="s">
         <v>72</v>
       </c>
       <c r="E15" s="2" t="s">
@@ -1127,10 +1137,10 @@
       <c r="B16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="7" t="s">
         <v>73</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -1144,10 +1154,10 @@
       <c r="B17" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="7" t="s">
         <v>74</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -1161,10 +1171,10 @@
       <c r="B18" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="7" t="s">
         <v>75</v>
       </c>
       <c r="E18" s="2" t="s">
@@ -1178,27 +1188,27 @@
       <c r="B19" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="7" t="s">
         <v>77</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="40" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="7" t="s">
         <v>101</v>
       </c>
       <c r="E20" s="2" t="s">
@@ -1212,27 +1222,27 @@
       <c r="B21" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="7" t="s">
         <v>78</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="40" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="7" t="s">
         <v>103</v>
       </c>
       <c r="E22" s="2" t="s">
@@ -1246,10 +1256,10 @@
       <c r="B23" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="7" t="s">
         <v>79</v>
       </c>
       <c r="E23" s="2" t="s">
@@ -1263,10 +1273,10 @@
       <c r="B24" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="7" t="s">
         <v>80</v>
       </c>
       <c r="E24" s="2" t="s">
@@ -1280,10 +1290,10 @@
       <c r="B25" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="7" t="s">
         <v>81</v>
       </c>
       <c r="E25" s="2" t="s">
@@ -1297,10 +1307,10 @@
       <c r="B26" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="7" t="s">
         <v>82</v>
       </c>
       <c r="E26" s="2" t="s">
@@ -1314,10 +1324,10 @@
       <c r="B27" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="7" t="s">
         <v>83</v>
       </c>
       <c r="E27" s="2" t="s">
@@ -1331,10 +1341,10 @@
       <c r="B28" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="7" t="s">
         <v>84</v>
       </c>
       <c r="E28" s="2" t="s">

</xml_diff>